<commit_message>
VGP Garden Fabrics 수정
#846
</commit_message>
<xml_diff>
--- a/Data/VGP/VGP Garden Fabrics - 2007062162/2007062162.xlsx
+++ b/Data/VGP/VGP Garden Fabrics - 2007062162/2007062162.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\VGP\VGP Garden Fabrics - 2007062162\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EC4FE5-D46B-49B2-A89E-AE0030204A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9839C670-0DCC-4BC9-A511-75B8D93C45F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,7 +558,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="363">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1412,280 +1412,282 @@
     <t>방직</t>
   </si>
   <si>
+    <t>꽃에서 섬유를 추출하여 옷을 만드는 데 쓸 수 있습니다.</t>
+  </si>
+  <si>
+    <t>아마풀</t>
+  </si>
+  <si>
+    <t>재봉틀을 사용하여 원료를 유용한 천으로 만들 수 있습니다.</t>
+  </si>
+  <si>
+    <t>전기 베틀</t>
+  </si>
+  <si>
+    <t>베틀</t>
+  </si>
+  <si>
+    <t>부드럽고 가벼우며 단열에 매우 좋습니다. 털옷은 극한의 조건에서도 신체를 따뜻하게 유지해줍니다.</t>
+  </si>
+  <si>
+    <t>옷을 만드는데 쓰입니다. 부드럽고, 가벼우며 튼튼합니다.</t>
+  </si>
+  <si>
+    <t>아마 원단</t>
+  </si>
+  <si>
+    <t>삼베</t>
+  </si>
+  <si>
+    <t>담배를 피우는 물건들로 짠 옷감이라는 것을 이 옷을 입은 사람들이 좋은 생각이라고 생각하겠습니까?</t>
+  </si>
+  <si>
+    <t>플라스틸을 실처럼 엮여 만든 플라스틸가닥으로 고급 천을 만드는 데 사용됩니다.</t>
+  </si>
+  <si>
+    <t>플라스틸가닥</t>
+  </si>
+  <si>
+    <t>가공되지 않은 악마가닥으로 옷을 만들거나 거래에 사용됩니다.</t>
+  </si>
+  <si>
+    <t>악마가닥</t>
+  </si>
+  <si>
+    <t>가공되지 않은 아마로 옷을 만들거나 거래에 사용됩니다.</t>
+  </si>
+  <si>
+    <t>아마 섬유</t>
+  </si>
+  <si>
+    <t>가공되지 않은 목화로 옷을 만들거나 거래에 사용됩니다.</t>
+  </si>
+  <si>
+    <t>목화 섬유</t>
+  </si>
+  <si>
+    <t>미가공 직물</t>
+  </si>
+  <si>
+    <t>초경조직 천을 짜는 방법을 연구합니다.\n베틀에서 초경조직 천을 만들 수 있습니다.</t>
+  </si>
+  <si>
+    <t>초경조직 천</t>
+  </si>
+  <si>
+    <t>합성원단을 짜는 방법을 연구합니다.\n베틀에서 합성원단을 만들 수 있습니다.</t>
+  </si>
+  <si>
+    <t>합성원단</t>
+  </si>
+  <si>
+    <t>의복에 사용된 원단을 추출합니다.</t>
+  </si>
+  <si>
+    <t>의류 재활용</t>
+  </si>
+  <si>
+    <t>플라스틸가닥 방직하는 중</t>
+  </si>
+  <si>
+    <t>천 방직하는 중</t>
+  </si>
+  <si>
+    <t>아마 원단 방직하는 중</t>
+  </si>
+  <si>
+    <t>삼베 방직하는 중</t>
+  </si>
+  <si>
+    <t>누더기 만드는 중</t>
+  </si>
+  <si>
+    <t>합성원단 방직하는 중</t>
+  </si>
+  <si>
+    <t>합성원단 직조 중</t>
+  </si>
+  <si>
+    <t>악마가닥 천 방직하는 중</t>
+  </si>
+  <si>
+    <t>초경조직 천 직조 중</t>
+  </si>
+  <si>
+    <t>털실 혼방 중</t>
+  </si>
+  <si>
+    <t>천 짜는 중</t>
+  </si>
+  <si>
+    <t>의복 재활용 중</t>
+  </si>
+  <si>
+    <t>목화 섬유로 천을 짜냅니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아마풀로 아마 원단을 만듭니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다양한 가죽 부스러기를 하나로 결합하여 조잡한 가죽 누더기를 만듭니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대마의 인피섬유에서 삼베를 짜냅니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플라스틸을 실처럼 엮여 플라스틸가닥을 만들며, 고급 천을 만드는 데 사용됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>목화, 아마풀, 플라스틸가닥을 합성하여 합성원단을 만듭니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>악마가닥을 옷감으로 사용할 수 있게 가공합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>목화, 아마풀, 악마가닥, 플라스틸가닥을 합성하여 초경조직 천을 만듭니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 털실을 혼합하여 혼방 털실을 방직합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 털실을 혼합하여 혼방털실을 방직합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 직물을 이용해 천을 만듭니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>혼방 털실</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>천 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeClothHand.label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아마 원단 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeLinenHand.label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>간이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>제작</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레시피</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼베 제작</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아마 원단 제작</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>천 제작</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeCloth.label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecipeDef+MakeLinen.label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>천 x5 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아마 원단 x7 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>누더기 x4 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼베 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼베 x5 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>합성원단 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>합성원단 x4 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>악마가닥 천 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>악마가닥 천 x5 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초경조직 천 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초경조직 천 x4 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>혼방 털실 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>혼방 털실 x5 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 직물로 천 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 직물로 천 x4 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플라스틸가닥 만들기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닐라 번역</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>베틀로 짜기</t>
-  </si>
-  <si>
-    <t>꽃에서 섬유를 추출하여 옷을 만드는 데 쓸 수 있습니다.</t>
-  </si>
-  <si>
-    <t>아마풀</t>
-  </si>
-  <si>
-    <t>재봉틀을 사용하여 원료를 유용한 천으로 만들 수 있습니다.</t>
-  </si>
-  <si>
-    <t>전기 베틀</t>
-  </si>
-  <si>
-    <t>베틀</t>
-  </si>
-  <si>
-    <t>부드럽고 가벼우며 단열에 매우 좋습니다. 털옷은 극한의 조건에서도 신체를 따뜻하게 유지해줍니다.</t>
-  </si>
-  <si>
-    <t>옷을 만드는데 쓰입니다. 부드럽고, 가벼우며 튼튼합니다.</t>
-  </si>
-  <si>
-    <t>아마 원단</t>
-  </si>
-  <si>
-    <t>삼베</t>
-  </si>
-  <si>
-    <t>담배를 피우는 물건들로 짠 옷감이라는 것을 이 옷을 입은 사람들이 좋은 생각이라고 생각하겠습니까?</t>
-  </si>
-  <si>
-    <t>플라스틸을 실처럼 엮여 만든 플라스틸가닥으로 고급 천을 만드는 데 사용됩니다.</t>
-  </si>
-  <si>
-    <t>플라스틸가닥</t>
-  </si>
-  <si>
-    <t>가공되지 않은 악마가닥으로 옷을 만들거나 거래에 사용됩니다.</t>
-  </si>
-  <si>
-    <t>악마가닥</t>
-  </si>
-  <si>
-    <t>가공되지 않은 아마로 옷을 만들거나 거래에 사용됩니다.</t>
-  </si>
-  <si>
-    <t>아마 섬유</t>
-  </si>
-  <si>
-    <t>가공되지 않은 목화로 옷을 만들거나 거래에 사용됩니다.</t>
-  </si>
-  <si>
-    <t>목화 섬유</t>
-  </si>
-  <si>
-    <t>미가공 직물</t>
-  </si>
-  <si>
-    <t>채소밭</t>
-  </si>
-  <si>
-    <t>초경조직 천을 짜는 방법을 연구합니다.\n베틀에서 초경조직 천을 만들 수 있습니다.</t>
-  </si>
-  <si>
-    <t>초경조직 천</t>
-  </si>
-  <si>
-    <t>합성원단을 짜는 방법을 연구합니다.\n베틀에서 합성원단을 만들 수 있습니다.</t>
-  </si>
-  <si>
-    <t>합성원단</t>
-  </si>
-  <si>
-    <t>의복에 사용된 원단을 추출합니다.</t>
-  </si>
-  <si>
-    <t>의류 재활용</t>
-  </si>
-  <si>
-    <t>플라스틸가닥 방직하는 중</t>
-  </si>
-  <si>
-    <t>천 방직하는 중</t>
-  </si>
-  <si>
-    <t>아마 원단 방직하는 중</t>
-  </si>
-  <si>
-    <t>삼베 방직하는 중</t>
-  </si>
-  <si>
-    <t>누더기 만드는 중</t>
-  </si>
-  <si>
-    <t>합성원단 방직하는 중</t>
-  </si>
-  <si>
-    <t>합성원단 직조 중</t>
-  </si>
-  <si>
-    <t>악마가닥 천 방직하는 중</t>
-  </si>
-  <si>
-    <t>초경조직 천 직조 중</t>
-  </si>
-  <si>
-    <t>털실 혼방 중</t>
-  </si>
-  <si>
-    <t>천 짜는 중</t>
-  </si>
-  <si>
-    <t>의복 재활용 중</t>
-  </si>
-  <si>
-    <t>목화 섬유로 천을 짜냅니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>아마풀로 아마 원단을 만듭니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다양한 가죽 부스러기를 하나로 결합하여 조잡한 가죽 누더기를 만듭니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>대마의 인피섬유에서 삼베를 짜냅니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>플라스틸을 실처럼 엮여 플라스틸가닥을 만들며, 고급 천을 만드는 데 사용됩니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>목화, 아마풀, 플라스틸가닥을 합성하여 합성원단을 만듭니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>악마가닥을 옷감으로 사용할 수 있게 가공합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>목화, 아마풀, 악마가닥, 플라스틸가닥을 합성하여 초경조직 천을 만듭니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다른 털실을 혼합하여 혼방 털실을 방직합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다른 털실을 혼합하여 혼방털실을 방직합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다른 직물을 이용해 천을 만듭니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>혼방 털실</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>천 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecipeDef+MakeClothHand.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>아마 원단 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecipeDef+MakeLinenHand.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>간이</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>레시피</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삼베 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>아마 원단 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>천 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecipeDef+MakeCloth.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>RecipeDef+MakeLinen.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>천 x5 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>아마 원단 x7 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>누더기 x4 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삼베 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삼베 x5 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>합성원단 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>합성원단 x4 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>악마가닥 천 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>악마가닥 천 x5 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>초경조직 천 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>초경조직 천 x4 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>혼방 털실 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>혼방 털실 x5 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다른 직물로 천 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다른 직물로 천 x4 만들기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>플라스틸가닥 만들기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2105,7 +2107,7 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2116,7 +2118,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.1796875" style="1" customWidth="1"/>
     <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -2141,7 +2144,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -2154,10 +2157,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H2" s="5"/>
     </row>
@@ -2176,10 +2179,10 @@
         <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -2198,16 +2201,16 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
@@ -2220,7 +2223,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="5"/>
@@ -2240,7 +2243,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="5"/>
@@ -2260,7 +2263,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="5"/>
@@ -2279,7 +2282,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5"/>
@@ -2298,7 +2301,7 @@
         <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="5"/>
@@ -2318,14 +2321,14 @@
         <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>6</v>
@@ -2338,7 +2341,7 @@
         <v>33</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H11" s="5"/>
     </row>
@@ -2357,7 +2360,7 @@
         <v>36</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
@@ -2375,7 +2378,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
@@ -2393,7 +2396,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -2411,7 +2414,7 @@
         <v>44</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
@@ -2429,12 +2432,12 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>6</v>
@@ -2447,10 +2450,10 @@
         <v>48</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
@@ -2465,10 +2468,10 @@
         <v>51</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
@@ -2483,10 +2486,10 @@
         <v>22</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
@@ -2501,10 +2504,10 @@
         <v>56</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>57</v>
       </c>
@@ -2519,10 +2522,10 @@
         <v>59</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
@@ -2537,10 +2540,10 @@
         <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -2555,10 +2558,10 @@
         <v>64</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>65</v>
       </c>
@@ -2573,10 +2576,13 @@
         <v>67</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+        <v>323</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>68</v>
       </c>
@@ -2591,10 +2597,11 @@
         <v>70</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+        <v>313</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>71</v>
       </c>
@@ -2609,10 +2616,10 @@
         <v>73</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>74</v>
       </c>
@@ -2627,10 +2634,10 @@
         <v>28</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>76</v>
       </c>
@@ -2645,10 +2652,10 @@
         <v>31</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>78</v>
       </c>
@@ -2663,10 +2670,10 @@
         <v>80</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>81</v>
       </c>
@@ -2681,10 +2688,10 @@
         <v>83</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>84</v>
       </c>
@@ -2699,10 +2706,10 @@
         <v>31</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>86</v>
       </c>
@@ -2717,7 +2724,7 @@
         <v>88</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -2735,7 +2742,7 @@
         <v>91</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -2753,7 +2760,7 @@
         <v>94</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -2771,7 +2778,7 @@
         <v>97</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -2789,7 +2796,7 @@
         <v>100</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -2807,7 +2814,7 @@
         <v>103</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -2825,7 +2832,7 @@
         <v>106</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
@@ -2843,7 +2850,7 @@
         <v>109</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -2861,7 +2868,7 @@
         <v>103</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -2879,7 +2886,7 @@
         <v>114</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -2897,7 +2904,7 @@
         <v>117</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -2915,7 +2922,7 @@
         <v>120</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -2933,7 +2940,7 @@
         <v>123</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
@@ -2951,7 +2958,7 @@
         <v>126</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -2969,7 +2976,7 @@
         <v>120</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -2987,7 +2994,7 @@
         <v>131</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -3005,7 +3012,7 @@
         <v>134</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
@@ -3023,7 +3030,7 @@
         <v>137</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
@@ -3041,7 +3048,7 @@
         <v>140</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
@@ -3059,7 +3066,7 @@
         <v>143</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -3077,7 +3084,7 @@
         <v>137</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -3095,7 +3102,7 @@
         <v>148</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
@@ -3113,7 +3120,7 @@
         <v>151</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
@@ -3131,7 +3138,7 @@
         <v>154</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
@@ -3149,7 +3156,7 @@
         <v>157</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
@@ -3167,7 +3174,7 @@
         <v>160</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
@@ -3185,7 +3192,7 @@
         <v>154</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
@@ -3203,7 +3210,7 @@
         <v>165</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
@@ -3221,7 +3228,7 @@
         <v>168</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
@@ -3239,7 +3246,7 @@
         <v>171</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
@@ -3257,7 +3264,7 @@
         <v>174</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
@@ -3275,7 +3282,7 @@
         <v>177</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
@@ -3293,7 +3300,7 @@
         <v>171</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -3311,7 +3318,7 @@
         <v>182</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
@@ -3329,7 +3336,7 @@
         <v>185</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
@@ -3347,7 +3354,7 @@
         <v>188</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
@@ -3364,7 +3371,7 @@
         <v>192</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
@@ -3381,7 +3388,7 @@
         <v>195</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
@@ -3398,41 +3405,43 @@
         <v>198</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="D71" s="2"/>
+      <c r="E71" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>305</v>
+      <c r="F71" s="2" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="D72" s="2"/>
+      <c r="E72" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>304</v>
+      <c r="F72" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
@@ -3449,7 +3458,7 @@
         <v>209</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
@@ -3466,7 +3475,7 @@
         <v>213</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
@@ -3483,7 +3492,7 @@
         <v>216</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
@@ -3500,7 +3509,7 @@
         <v>219</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
@@ -3517,7 +3526,7 @@
         <v>222</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
@@ -3534,7 +3543,7 @@
         <v>225</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
@@ -3551,7 +3560,7 @@
         <v>228</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
@@ -3568,7 +3577,7 @@
         <v>231</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
@@ -3585,7 +3594,7 @@
         <v>234</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
@@ -3602,7 +3611,7 @@
         <v>237</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
@@ -3619,7 +3628,7 @@
         <v>240</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
@@ -3636,7 +3645,7 @@
         <v>243</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
@@ -3653,7 +3662,7 @@
         <v>246</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
@@ -3670,7 +3679,7 @@
         <v>249</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
@@ -3687,7 +3696,7 @@
         <v>252</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
@@ -3704,7 +3713,7 @@
         <v>255</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
@@ -3721,7 +3730,7 @@
         <v>258</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
@@ -3738,7 +3747,7 @@
         <v>261</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
@@ -3755,7 +3764,7 @@
         <v>264</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
@@ -3772,7 +3781,7 @@
         <v>261</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
@@ -3789,7 +3798,7 @@
         <v>269</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
@@ -3806,7 +3815,7 @@
         <v>272</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
@@ -3823,7 +3832,7 @@
         <v>276</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>284</v>
+        <v>362</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">

</xml_diff>